<commit_message>
Modulo4[feat]: new img compartion
</commit_message>
<xml_diff>
--- a/documentation/Dados_teste.xlsx
+++ b/documentation/Dados_teste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\luan\Projects\Sistemas_Operacionais\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F128D1E-D43B-4964-8F7C-A608A5D14B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A65A37-7728-4E1A-AA0B-8F8F96E99EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70F01DA2-7212-451F-B3A6-51E387577920}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="78">
-  <si>
-    <t>First Job First Service (FIFO)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="85">
   <si>
     <t>Teste</t>
   </si>
@@ -268,6 +265,30 @@
   </si>
   <si>
     <t>FIFO</t>
+  </si>
+  <si>
+    <t>First Come First Service (FIFO)</t>
+  </si>
+  <si>
+    <t>Preemptivo sem MMU</t>
+  </si>
+  <si>
+    <t>Preemptivo com MMU</t>
+  </si>
+  <si>
+    <t>27 ms</t>
+  </si>
+  <si>
+    <t>26 ms</t>
+  </si>
+  <si>
+    <t>31 ms</t>
+  </si>
+  <si>
+    <t>25 ms</t>
+  </si>
+  <si>
+    <t>24 ms</t>
   </si>
 </sst>
 </file>
@@ -295,11 +316,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF404040"/>
-      <name val="Segoe UI"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -322,16 +344,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -339,6 +355,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364D5E8E-4553-4C4C-8804-F3A2B2FC944C}">
-  <dimension ref="B2:X26"/>
+  <dimension ref="B2:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="78" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14:V19"/>
+    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,1020 +702,1156 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
       <c r="S2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
     </row>
     <row r="3" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
       <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
       <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
-        <v>3</v>
-      </c>
       <c r="N3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>2</v>
       </c>
-      <c r="P3" t="s">
-        <v>3</v>
-      </c>
       <c r="S3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="5">
+        <v>69</v>
+      </c>
+      <c r="T3" s="3">
         <v>75.8</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="3">
         <v>13.9</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="3">
         <v>61.9</v>
       </c>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
     </row>
     <row r="4" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T4" s="5">
+        <v>70</v>
+      </c>
+      <c r="T4" s="3">
         <v>77</v>
       </c>
-      <c r="U4" s="5">
+      <c r="U4" s="3">
         <v>14.7</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="3">
         <v>62.3</v>
       </c>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
     </row>
     <row r="5" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
       <c r="N5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T5" s="5">
+        <v>71</v>
+      </c>
+      <c r="T5" s="3">
         <v>84</v>
       </c>
-      <c r="U5" s="5">
+      <c r="U5" s="3">
         <v>14.3</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="3">
         <v>69.7</v>
       </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
     </row>
     <row r="6" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T6" s="5">
+        <v>72</v>
+      </c>
+      <c r="T6" s="3">
         <v>79.8</v>
       </c>
-      <c r="U6" s="5">
+      <c r="U6" s="3">
         <v>14.6</v>
       </c>
-      <c r="V6" s="5">
+      <c r="V6" s="3">
         <v>65.2</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
       <c r="J7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" t="s">
         <v>23</v>
-      </c>
-      <c r="N7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O7" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" t="s">
         <v>51</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P12" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" t="s">
-        <v>33</v>
-      </c>
-      <c r="P9" t="s">
-        <v>53</v>
-      </c>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" t="s">
-        <v>47</v>
-      </c>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" t="s">
-        <v>23</v>
-      </c>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="2:24" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" t="s">
-        <v>28</v>
-      </c>
-      <c r="S12" s="3"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" t="s">
-        <v>4</v>
-      </c>
-      <c r="P13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="N15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="N15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15" t="s">
+        <v>74</v>
+      </c>
+      <c r="U15" t="s">
         <v>75</v>
       </c>
-      <c r="U15" t="s">
-        <v>76</v>
-      </c>
       <c r="V15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
       <c r="F16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
         <v>20</v>
       </c>
-      <c r="H16" t="s">
-        <v>21</v>
-      </c>
       <c r="J16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" t="s">
         <v>20</v>
       </c>
-      <c r="L16" t="s">
-        <v>21</v>
-      </c>
       <c r="N16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" t="s">
         <v>20</v>
       </c>
-      <c r="P16" t="s">
-        <v>21</v>
-      </c>
       <c r="S16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="T16" s="5">
+        <v>76</v>
+      </c>
+      <c r="T16" s="3">
         <v>75.8</v>
       </c>
-      <c r="U16" s="5">
+      <c r="U16" s="3">
         <v>38.1</v>
       </c>
-      <c r="V16" s="5">
+      <c r="V16" s="3">
         <v>37.700000000000003</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" t="s">
+        <v>48</v>
+      </c>
+      <c r="P17" t="s">
         <v>61</v>
       </c>
-      <c r="J17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" t="s">
-        <v>57</v>
-      </c>
-      <c r="N17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O17" t="s">
-        <v>49</v>
-      </c>
-      <c r="P17" t="s">
-        <v>62</v>
-      </c>
       <c r="S17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="T17" s="5">
+        <v>70</v>
+      </c>
+      <c r="T17" s="3">
         <v>77</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17" s="3">
         <v>40.799999999999997</v>
       </c>
-      <c r="V17" s="5">
+      <c r="V17" s="3">
         <v>36.200000000000003</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="T18" s="5">
+        <v>71</v>
+      </c>
+      <c r="T18" s="3">
         <v>84</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="3">
         <v>40.9</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="3">
         <v>43.1</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T19" s="5">
+        <v>72</v>
+      </c>
+      <c r="T19" s="3">
         <v>79.8</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="3">
         <v>40.1</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="3">
         <v>39.700000000000003</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P20" t="s">
         <v>56</v>
-      </c>
-      <c r="J20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" t="s">
-        <v>58</v>
-      </c>
-      <c r="N20" t="s">
-        <v>11</v>
-      </c>
-      <c r="O20" t="s">
-        <v>50</v>
-      </c>
-      <c r="P20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" t="s">
-        <v>58</v>
-      </c>
-      <c r="N22" t="s">
-        <v>13</v>
-      </c>
-      <c r="O22" t="s">
-        <v>33</v>
-      </c>
       <c r="P22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25" t="s">
         <v>57</v>
       </c>
-      <c r="J25" t="s">
-        <v>16</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" t="s">
-        <v>58</v>
-      </c>
       <c r="N25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" t="s">
+        <v>3</v>
+      </c>
+      <c r="P26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
         <v>55</v>
       </c>
-      <c r="F26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
-      <c r="H26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" t="s">
-        <v>46</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
         <v>57</v>
       </c>
-      <c r="N26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" t="s">
-        <v>64</v>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="J15:L15"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>